<commit_message>
Now all finished including the report, but im going to redo all tables...
</commit_message>
<xml_diff>
--- a/Tests/TestCases_Preprocessing/17TestCut2SeuilFunc1+addmipstart/pre_cut2_seuil_func_mipstart.xlsx
+++ b/Tests/TestCases_Preprocessing/17TestCut2SeuilFunc1+addmipstart/pre_cut2_seuil_func_mipstart.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\PFE\MyWork\PFE\Others\TestCuts\17TestCut2SeuilFunc1+addmipstart\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\PFE\MyWork\PFE\Tests\TestCases_Preprocessing\17TestCut2SeuilFunc1+addmipstart\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2607,11 +2607,11 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="9"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="9"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2935,8 +2935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N104" activeCellId="1" sqref="I50:I104 N50:N104"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A50" sqref="A1:XFD50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2988,7 +2988,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -3035,7 +3035,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="3" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -3082,7 +3082,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -3129,7 +3129,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -3176,7 +3176,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="6" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -3223,7 +3223,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="7" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -3270,7 +3270,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="8" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -3317,7 +3317,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -3364,7 +3364,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="10" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -3411,7 +3411,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -3458,7 +3458,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="12" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>48</v>
       </c>
@@ -3505,7 +3505,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="13" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -3552,7 +3552,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="14" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>54</v>
       </c>
@@ -3599,7 +3599,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="15" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -3646,7 +3646,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="16" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>58</v>
       </c>
@@ -3693,7 +3693,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="17" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>60</v>
       </c>
@@ -3740,7 +3740,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="18" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>63</v>
       </c>
@@ -3787,7 +3787,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="19" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>66</v>
       </c>
@@ -3834,7 +3834,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="20" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>69</v>
       </c>
@@ -3881,7 +3881,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>73</v>
       </c>
@@ -3928,7 +3928,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>78</v>
       </c>
@@ -3975,7 +3975,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="23" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>82</v>
       </c>
@@ -4022,7 +4022,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="24" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>86</v>
       </c>
@@ -4069,7 +4069,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>90</v>
       </c>
@@ -4116,7 +4116,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="26" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>94</v>
       </c>
@@ -4163,7 +4163,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="27" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>98</v>
       </c>
@@ -4210,7 +4210,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="28" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>102</v>
       </c>
@@ -4257,7 +4257,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="29" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>106</v>
       </c>
@@ -4304,7 +4304,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="30" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>110</v>
       </c>
@@ -4351,7 +4351,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="31" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>114</v>
       </c>
@@ -4398,7 +4398,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="32" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>118</v>
       </c>
@@ -4445,7 +4445,7 @@
         <v>1332</v>
       </c>
     </row>
-    <row r="33" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>123</v>
       </c>
@@ -4492,7 +4492,7 @@
         <v>1968</v>
       </c>
     </row>
-    <row r="34" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>128</v>
       </c>
@@ -4539,7 +4539,7 @@
         <v>1764</v>
       </c>
     </row>
-    <row r="35" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>133</v>
       </c>
@@ -4586,7 +4586,7 @@
         <v>1764</v>
       </c>
     </row>
-    <row r="36" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>138</v>
       </c>
@@ -4633,7 +4633,7 @@
         <v>1632</v>
       </c>
     </row>
-    <row r="37" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>144</v>
       </c>
@@ -4680,7 +4680,7 @@
         <v>1596</v>
       </c>
     </row>
-    <row r="38" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>149</v>
       </c>
@@ -4727,7 +4727,7 @@
         <v>1956</v>
       </c>
     </row>
-    <row r="39" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>153</v>
       </c>
@@ -4774,7 +4774,7 @@
         <v>1764</v>
       </c>
     </row>
-    <row r="40" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>157</v>
       </c>
@@ -4821,7 +4821,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="41" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>162</v>
       </c>
@@ -4868,7 +4868,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="42" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>167</v>
       </c>
@@ -4915,7 +4915,7 @@
         <v>1704</v>
       </c>
     </row>
-    <row r="43" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>172</v>
       </c>
@@ -4962,7 +4962,7 @@
         <v>1320</v>
       </c>
     </row>
-    <row r="44" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>176</v>
       </c>
@@ -5009,7 +5009,7 @@
         <v>1560</v>
       </c>
     </row>
-    <row r="45" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>180</v>
       </c>
@@ -5056,7 +5056,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="46" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>183</v>
       </c>
@@ -5103,7 +5103,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="47" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>187</v>
       </c>
@@ -5150,7 +5150,7 @@
         <v>1512</v>
       </c>
     </row>
-    <row r="48" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>192</v>
       </c>
@@ -5197,7 +5197,7 @@
         <v>1920</v>
       </c>
     </row>
-    <row r="49" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>196</v>
       </c>
@@ -6209,7 +6209,7 @@
       <c r="H70">
         <v>1</v>
       </c>
-      <c r="I70" s="13" t="s">
+      <c r="I70" s="12" t="s">
         <v>303</v>
       </c>
       <c r="J70">
@@ -6256,7 +6256,7 @@
       <c r="H71">
         <v>1</v>
       </c>
-      <c r="I71" s="13" t="s">
+      <c r="I71" s="12" t="s">
         <v>306</v>
       </c>
       <c r="J71">
@@ -6303,7 +6303,7 @@
       <c r="H72">
         <v>1</v>
       </c>
-      <c r="I72" s="12" t="s">
+      <c r="I72" s="11" t="s">
         <v>314</v>
       </c>
       <c r="J72">
@@ -6444,7 +6444,7 @@
       <c r="H75">
         <v>1</v>
       </c>
-      <c r="I75" s="13" t="s">
+      <c r="I75" s="12" t="s">
         <v>330</v>
       </c>
       <c r="J75">
@@ -6491,7 +6491,7 @@
       <c r="H76">
         <v>1</v>
       </c>
-      <c r="I76" s="13" t="s">
+      <c r="I76" s="12" t="s">
         <v>336</v>
       </c>
       <c r="J76">
@@ -6585,7 +6585,7 @@
       <c r="H78">
         <v>1</v>
       </c>
-      <c r="I78" s="12" t="s">
+      <c r="I78" s="11" t="s">
         <v>347</v>
       </c>
       <c r="J78">
@@ -6679,7 +6679,7 @@
       <c r="H80">
         <v>1</v>
       </c>
-      <c r="I80" s="12" t="s">
+      <c r="I80" s="11" t="s">
         <v>358</v>
       </c>
       <c r="J80">
@@ -6914,7 +6914,7 @@
       <c r="H85">
         <v>1</v>
       </c>
-      <c r="I85" s="13" t="s">
+      <c r="I85" s="12" t="s">
         <v>384</v>
       </c>
       <c r="J85">
@@ -7008,7 +7008,7 @@
       <c r="H87">
         <v>1</v>
       </c>
-      <c r="I87" s="12" t="s">
+      <c r="I87" s="11" t="s">
         <v>395</v>
       </c>
       <c r="J87">
@@ -7055,7 +7055,7 @@
       <c r="H88">
         <v>1</v>
       </c>
-      <c r="I88" s="12" t="s">
+      <c r="I88" s="11" t="s">
         <v>401</v>
       </c>
       <c r="J88">
@@ -7102,7 +7102,7 @@
       <c r="H89">
         <v>1</v>
       </c>
-      <c r="I89" s="13" t="s">
+      <c r="I89" s="12" t="s">
         <v>407</v>
       </c>
       <c r="J89">
@@ -7196,7 +7196,7 @@
       <c r="H91">
         <v>1</v>
       </c>
-      <c r="I91" s="13" t="s">
+      <c r="I91" s="12" t="s">
         <v>418</v>
       </c>
       <c r="J91">
@@ -7243,7 +7243,7 @@
       <c r="H92">
         <v>1</v>
       </c>
-      <c r="I92" s="12" t="s">
+      <c r="I92" s="11" t="s">
         <v>421</v>
       </c>
       <c r="J92">
@@ -7290,7 +7290,7 @@
       <c r="H93">
         <v>1</v>
       </c>
-      <c r="I93" s="12" t="s">
+      <c r="I93" s="11" t="s">
         <v>428</v>
       </c>
       <c r="J93">
@@ -7337,7 +7337,7 @@
       <c r="H94">
         <v>1</v>
       </c>
-      <c r="I94" s="13" t="s">
+      <c r="I94" s="12" t="s">
         <v>434</v>
       </c>
       <c r="J94">
@@ -7478,7 +7478,7 @@
       <c r="H97">
         <v>1</v>
       </c>
-      <c r="I97" s="12" t="s">
+      <c r="I97" s="11" t="s">
         <v>450</v>
       </c>
       <c r="J97">
@@ -7525,7 +7525,7 @@
       <c r="H98">
         <v>1</v>
       </c>
-      <c r="I98" s="12" t="s">
+      <c r="I98" s="11" t="s">
         <v>456</v>
       </c>
       <c r="J98">
@@ -7572,7 +7572,7 @@
       <c r="H99">
         <v>1</v>
       </c>
-      <c r="I99" s="13" t="s">
+      <c r="I99" s="12" t="s">
         <v>462</v>
       </c>
       <c r="J99">
@@ -7666,7 +7666,7 @@
       <c r="H101">
         <v>1</v>
       </c>
-      <c r="I101" s="13" t="s">
+      <c r="I101" s="12" t="s">
         <v>473</v>
       </c>
       <c r="J101">
@@ -7760,7 +7760,7 @@
       <c r="H103">
         <v>1</v>
       </c>
-      <c r="I103" s="13" t="s">
+      <c r="I103" s="12" t="s">
         <v>484</v>
       </c>
       <c r="J103">
@@ -9389,12 +9389,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H104"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34:H39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
     <col min="3" max="3" width="19.85546875" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="8"/>
   </cols>
@@ -9922,9 +9923,9 @@
         <f t="shared" si="0"/>
         <v>8.1447963800905043</v>
       </c>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -11642,9 +11643,9 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C39" s="9"/>

</xml_diff>